<commit_message>
some progress on designating dabom site operations
</commit_message>
<xml_diff>
--- a/output/iptds_operations/dabom_site_operations_2024-08-08.xlsx
+++ b/output/iptds_operations/dabom_site_operations_2024-08-08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\output\iptds_operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCC1C17-3852-4C26-B29B-D0F71EECDDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8144675-4B7D-4131-908B-4F30C73BB279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -957,8 +957,8 @@
   <dimension ref="A1:N3220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1049" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1076" sqref="M1076"/>
+      <pane ySplit="1" topLeftCell="A1641" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1649" sqref="M1649"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36430,6 +36430,9 @@
       <c r="L1076" t="b">
         <v>1</v>
       </c>
+      <c r="M1076" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1077" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1077" t="s">
@@ -36457,6 +36460,9 @@
         <v>0</v>
       </c>
       <c r="L1077" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1077" t="b">
         <v>1</v>
       </c>
     </row>
@@ -36982,6 +36988,9 @@
       <c r="L1091" t="b">
         <v>1</v>
       </c>
+      <c r="M1091" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1092" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1092" t="s">
@@ -37014,6 +37023,9 @@
       <c r="L1092" t="b">
         <v>1</v>
       </c>
+      <c r="M1092" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1093" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1093" t="s">
@@ -37526,6 +37538,9 @@
       <c r="L1105" t="b">
         <v>1</v>
       </c>
+      <c r="M1105" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1106" t="s">
@@ -37553,6 +37568,9 @@
         <v>0</v>
       </c>
       <c r="L1106" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1106" t="b">
         <v>1</v>
       </c>
     </row>
@@ -38078,6 +38096,9 @@
       <c r="L1120" t="b">
         <v>1</v>
       </c>
+      <c r="M1120" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1121" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1121" t="s">
@@ -38110,6 +38131,9 @@
       <c r="L1121" t="b">
         <v>1</v>
       </c>
+      <c r="M1121" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1122" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1122" t="s">
@@ -38622,6 +38646,9 @@
       <c r="L1134" t="b">
         <v>1</v>
       </c>
+      <c r="M1134" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1135" t="s">
@@ -38652,6 +38679,9 @@
         <v>0</v>
       </c>
       <c r="L1135" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1135" t="b">
         <v>1</v>
       </c>
     </row>
@@ -39204,6 +39234,9 @@
       <c r="L1149" t="b">
         <v>1</v>
       </c>
+      <c r="M1149" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1150" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1150" t="s">
@@ -39236,6 +39269,9 @@
       <c r="L1150" t="b">
         <v>1</v>
       </c>
+      <c r="M1150" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1151" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1151" t="s">
@@ -39940,6 +39976,9 @@
       <c r="L1169" t="b">
         <v>1</v>
       </c>
+      <c r="M1169" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1170" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1170" t="s">
@@ -39978,6 +40017,9 @@
       <c r="L1170" t="b">
         <v>1</v>
       </c>
+      <c r="M1170" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1171" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1171" t="s">
@@ -40016,6 +40058,9 @@
       <c r="L1171" t="b">
         <v>1</v>
       </c>
+      <c r="M1171" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1172" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1172" t="s">
@@ -40054,6 +40099,9 @@
       <c r="L1172" t="b">
         <v>1</v>
       </c>
+      <c r="M1172" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1173" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1173" t="s">
@@ -40092,6 +40140,9 @@
       <c r="L1173" t="b">
         <v>1</v>
       </c>
+      <c r="M1173" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1174" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1174" t="s">
@@ -40130,6 +40181,9 @@
       <c r="L1174" t="b">
         <v>1</v>
       </c>
+      <c r="M1174" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1175" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1175" t="s">
@@ -40166,6 +40220,9 @@
         <v>0</v>
       </c>
       <c r="L1175" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1175" t="b">
         <v>1</v>
       </c>
     </row>
@@ -40203,6 +40260,9 @@
       <c r="L1176" t="b">
         <v>1</v>
       </c>
+      <c r="M1176" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1177" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1177" t="s">
@@ -40456,6 +40516,9 @@
       <c r="L1184" t="b">
         <v>1</v>
       </c>
+      <c r="M1184" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1185" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1185" t="s">
@@ -40494,6 +40557,9 @@
       <c r="L1185" t="b">
         <v>1</v>
       </c>
+      <c r="M1185" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1186" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1186" t="s">
@@ -40532,6 +40598,9 @@
       <c r="L1186" t="b">
         <v>1</v>
       </c>
+      <c r="M1186" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1187" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1187" t="s">
@@ -40570,6 +40639,9 @@
       <c r="L1187" t="b">
         <v>1</v>
       </c>
+      <c r="M1187" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1188" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1188" t="s">
@@ -40608,6 +40680,9 @@
       <c r="L1188" t="b">
         <v>1</v>
       </c>
+      <c r="M1188" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1189" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1189" t="s">
@@ -40646,6 +40721,9 @@
       <c r="L1189" t="b">
         <v>1</v>
       </c>
+      <c r="M1189" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1190" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1190" t="s">
@@ -40684,6 +40762,9 @@
       <c r="L1190" t="b">
         <v>1</v>
       </c>
+      <c r="M1190" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1191" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1191" t="s">
@@ -40935,6 +41016,9 @@
         <v>0</v>
       </c>
       <c r="L1198" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1198" t="b">
         <v>1</v>
       </c>
     </row>
@@ -41474,6 +41558,9 @@
       <c r="L1213" t="b">
         <v>1</v>
       </c>
+      <c r="M1213" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1214" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1214" t="s">
@@ -41512,6 +41599,9 @@
       <c r="L1214" t="b">
         <v>1</v>
       </c>
+      <c r="M1214" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1215" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1215" t="s">
@@ -41673,6 +41763,9 @@
       <c r="L1218" t="b">
         <v>1</v>
       </c>
+      <c r="M1218" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1219" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1219" t="s">
@@ -42070,6 +42163,9 @@
       </c>
       <c r="L1231" t="b">
         <v>1</v>
+      </c>
+      <c r="M1231" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1232" spans="1:13" x14ac:dyDescent="0.35">
@@ -42682,6 +42778,9 @@
       <c r="L1250" t="b">
         <v>1</v>
       </c>
+      <c r="M1250" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1251" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1251" t="s">
@@ -42714,6 +42813,9 @@
       <c r="L1251" t="b">
         <v>1</v>
       </c>
+      <c r="M1251" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1252" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1252" t="s">
@@ -42997,6 +43099,9 @@
       </c>
       <c r="L1258" t="b">
         <v>1</v>
+      </c>
+      <c r="M1258" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1259" spans="1:13" x14ac:dyDescent="0.35">
@@ -43270,6 +43375,9 @@
       <c r="L1265" t="b">
         <v>1</v>
       </c>
+      <c r="M1265" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1266" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1266" t="s">
@@ -43302,6 +43410,9 @@
       <c r="L1266" t="b">
         <v>1</v>
       </c>
+      <c r="M1266" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1267" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1267" t="s">
@@ -43586,6 +43697,9 @@
       <c r="L1273" t="b">
         <v>1</v>
       </c>
+      <c r="M1273" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1274" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1274" t="s">
@@ -43967,6 +44081,9 @@
       <c r="L1288" t="b">
         <v>0</v>
       </c>
+      <c r="M1288" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1289" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1289" t="s">
@@ -44022,6 +44139,9 @@
         <v>0</v>
       </c>
       <c r="L1291" t="b">
+        <v>0</v>
+      </c>
+      <c r="M1291" t="b">
         <v>0</v>
       </c>
     </row>
@@ -44041,6 +44161,9 @@
       <c r="L1292" t="b">
         <v>0</v>
       </c>
+      <c r="M1292" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1293" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1293" t="s">
@@ -44058,6 +44181,9 @@
       <c r="L1293" t="b">
         <v>0</v>
       </c>
+      <c r="M1293" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1294" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1294" t="s">
@@ -44075,6 +44201,9 @@
       <c r="L1294" t="b">
         <v>0</v>
       </c>
+      <c r="M1294" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1295" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1295" t="s">
@@ -44092,6 +44221,9 @@
       <c r="L1295" t="b">
         <v>0</v>
       </c>
+      <c r="M1295" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1296" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1296" t="s">
@@ -44109,6 +44241,9 @@
       <c r="L1296" t="b">
         <v>0</v>
       </c>
+      <c r="M1296" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1297" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1297" t="s">
@@ -44126,6 +44261,9 @@
       <c r="L1297" t="b">
         <v>0</v>
       </c>
+      <c r="M1297" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1298" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1298" t="s">
@@ -44144,7 +44282,7 @@
         <v>1</v>
       </c>
       <c r="M1298" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1299" spans="1:13" x14ac:dyDescent="0.35">
@@ -44163,6 +44301,9 @@
       <c r="L1299" t="b">
         <v>0</v>
       </c>
+      <c r="M1299" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1300" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1300" t="s">
@@ -44180,6 +44321,9 @@
       <c r="L1300" t="b">
         <v>0</v>
       </c>
+      <c r="M1300" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1301" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1301" t="s">
@@ -44197,6 +44341,9 @@
       <c r="L1301" t="b">
         <v>0</v>
       </c>
+      <c r="M1301" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1302" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1302" t="s">
@@ -44214,6 +44361,9 @@
       <c r="L1302" t="b">
         <v>0</v>
       </c>
+      <c r="M1302" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1303" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1303" t="s">
@@ -44231,6 +44381,9 @@
       <c r="L1303" t="b">
         <v>0</v>
       </c>
+      <c r="M1303" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1304" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1304" t="s">
@@ -44248,6 +44401,9 @@
       <c r="L1304" t="b">
         <v>0</v>
       </c>
+      <c r="M1304" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1305" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1305" t="s">
@@ -44265,6 +44421,9 @@
       <c r="L1305" t="b">
         <v>0</v>
       </c>
+      <c r="M1305" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1306" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1306" t="s">
@@ -44282,6 +44441,9 @@
       <c r="L1306" t="b">
         <v>0</v>
       </c>
+      <c r="M1306" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1307" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1307" t="s">
@@ -44299,6 +44461,9 @@
       <c r="L1307" t="b">
         <v>0</v>
       </c>
+      <c r="M1307" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1308" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1308" t="s">
@@ -44316,6 +44481,9 @@
       <c r="L1308" t="b">
         <v>0</v>
       </c>
+      <c r="M1308" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1309" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1309" t="s">
@@ -44333,6 +44501,9 @@
       <c r="L1309" t="b">
         <v>0</v>
       </c>
+      <c r="M1309" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1310" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1310" t="s">
@@ -44350,6 +44521,9 @@
       <c r="L1310" t="b">
         <v>0</v>
       </c>
+      <c r="M1310" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1311" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1311" t="s">
@@ -44367,6 +44541,9 @@
       <c r="L1311" t="b">
         <v>0</v>
       </c>
+      <c r="M1311" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1312" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1312" t="s">
@@ -44384,6 +44561,9 @@
       <c r="L1312" t="b">
         <v>0</v>
       </c>
+      <c r="M1312" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1313" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1313" t="s">
@@ -44401,6 +44581,9 @@
       <c r="L1313" t="b">
         <v>0</v>
       </c>
+      <c r="M1313" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1314" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1314" t="s">
@@ -44418,6 +44601,9 @@
       <c r="L1314" t="b">
         <v>0</v>
       </c>
+      <c r="M1314" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1315" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1315" t="s">
@@ -44435,6 +44621,9 @@
       <c r="L1315" t="b">
         <v>0</v>
       </c>
+      <c r="M1315" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1316" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1316" t="s">
@@ -44452,6 +44641,9 @@
       <c r="L1316" t="b">
         <v>0</v>
       </c>
+      <c r="M1316" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1317" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1317" t="s">
@@ -44469,6 +44661,9 @@
       <c r="L1317" t="b">
         <v>0</v>
       </c>
+      <c r="M1317" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1318" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1318" t="s">
@@ -44486,6 +44681,9 @@
       <c r="L1318" t="b">
         <v>0</v>
       </c>
+      <c r="M1318" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1319" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1319" t="s">
@@ -44503,6 +44701,9 @@
       <c r="L1319" t="b">
         <v>0</v>
       </c>
+      <c r="M1319" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1320" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1320" t="s">
@@ -44518,6 +44719,9 @@
         <v>0</v>
       </c>
       <c r="L1320" t="b">
+        <v>0</v>
+      </c>
+      <c r="M1320" t="b">
         <v>0</v>
       </c>
     </row>
@@ -44537,6 +44741,9 @@
       <c r="L1321" t="b">
         <v>0</v>
       </c>
+      <c r="M1321" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1322" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1322" t="s">
@@ -44554,6 +44761,9 @@
       <c r="L1322" t="b">
         <v>0</v>
       </c>
+      <c r="M1322" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1323" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1323" t="s">
@@ -44751,6 +44961,9 @@
       <c r="L1332" t="b">
         <v>0</v>
       </c>
+      <c r="M1332" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1333" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1333" t="s">
@@ -44768,6 +44981,9 @@
       <c r="L1333" t="b">
         <v>0</v>
       </c>
+      <c r="M1333" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1334" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1334" t="s">
@@ -44785,6 +45001,9 @@
       <c r="L1334" t="b">
         <v>0</v>
       </c>
+      <c r="M1334" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1335" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1335" t="s">
@@ -44802,6 +45021,9 @@
       <c r="L1335" t="b">
         <v>0</v>
       </c>
+      <c r="M1335" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1336" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1336" t="s">
@@ -44834,6 +45056,9 @@
       <c r="L1336" t="b">
         <v>1</v>
       </c>
+      <c r="M1336" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1337" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1337" t="s">
@@ -44866,6 +45091,9 @@
       <c r="L1337" t="b">
         <v>1</v>
       </c>
+      <c r="M1337" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1338" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1338" t="s">
@@ -44896,6 +45124,9 @@
         <v>0</v>
       </c>
       <c r="L1338" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1338" t="b">
         <v>1</v>
       </c>
     </row>
@@ -45293,6 +45524,9 @@
       <c r="L1351" t="b">
         <v>1</v>
       </c>
+      <c r="M1351" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1352" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1352" t="s">
@@ -45325,6 +45559,9 @@
       <c r="L1352" t="b">
         <v>1</v>
       </c>
+      <c r="M1352" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1353" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1353" t="s">
@@ -45357,6 +45594,9 @@
       <c r="L1353" t="b">
         <v>1</v>
       </c>
+      <c r="M1353" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1354" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1354" t="s">
@@ -45395,6 +45635,9 @@
       <c r="L1354" t="b">
         <v>1</v>
       </c>
+      <c r="M1354" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1355" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1355" t="s">
@@ -45723,6 +45966,9 @@
       <c r="L1365" t="b">
         <v>1</v>
       </c>
+      <c r="M1365" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1366" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1366" t="s">
@@ -45755,6 +46001,9 @@
       <c r="L1366" t="b">
         <v>1</v>
       </c>
+      <c r="M1366" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1367" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1367" t="s">
@@ -45787,6 +46036,9 @@
       <c r="L1367" t="b">
         <v>1</v>
       </c>
+      <c r="M1367" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1368" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1368" t="s">
@@ -45907,6 +46159,9 @@
       <c r="L1370" t="b">
         <v>1</v>
       </c>
+      <c r="M1370" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1371" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1371" t="s">
@@ -45939,6 +46194,9 @@
       <c r="L1371" t="b">
         <v>1</v>
       </c>
+      <c r="M1371" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1372" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1372" t="s">
@@ -45970,6 +46228,9 @@
       </c>
       <c r="L1372" t="b">
         <v>1</v>
+      </c>
+      <c r="M1372" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1373" spans="1:13" x14ac:dyDescent="0.35">
@@ -46322,6 +46583,9 @@
       <c r="L1381" t="b">
         <v>1</v>
       </c>
+      <c r="M1381" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1382" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1382" t="s">
@@ -46354,6 +46618,9 @@
       <c r="L1382" t="b">
         <v>1</v>
       </c>
+      <c r="M1382" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1383" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1383" t="s">
@@ -46509,6 +46776,9 @@
       <c r="L1386" t="b">
         <v>1</v>
       </c>
+      <c r="M1386" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1387" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1387" t="s">
@@ -46541,6 +46811,9 @@
       <c r="L1387" t="b">
         <v>1</v>
       </c>
+      <c r="M1387" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1388" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1388" t="s">
@@ -46579,6 +46852,9 @@
       <c r="L1388" t="b">
         <v>1</v>
       </c>
+      <c r="M1388" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1389" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1389" t="s">
@@ -46816,6 +47092,9 @@
       <c r="L1394" t="b">
         <v>1</v>
       </c>
+      <c r="M1394" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1395" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1395" t="s">
@@ -46848,6 +47127,9 @@
       <c r="L1395" t="b">
         <v>1</v>
       </c>
+      <c r="M1395" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1396" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1396" t="s">
@@ -46880,6 +47162,9 @@
       <c r="L1396" t="b">
         <v>1</v>
       </c>
+      <c r="M1396" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1397" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1397" t="s">
@@ -46959,6 +47244,9 @@
       <c r="L1398" t="b">
         <v>1</v>
       </c>
+      <c r="M1398" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1399" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1399" t="s">
@@ -46997,6 +47285,9 @@
       <c r="L1399" t="b">
         <v>1</v>
       </c>
+      <c r="M1399" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1400" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1400" t="s">
@@ -47029,6 +47320,9 @@
       <c r="L1400" t="b">
         <v>1</v>
       </c>
+      <c r="M1400" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1401" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1401" t="s">
@@ -47067,6 +47361,9 @@
       <c r="L1401" t="b">
         <v>1</v>
       </c>
+      <c r="M1401" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1402" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1402" t="s">
@@ -47105,6 +47402,9 @@
       <c r="L1402" t="b">
         <v>1</v>
       </c>
+      <c r="M1402" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1403" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1403" t="s">
@@ -47136,6 +47436,9 @@
       </c>
       <c r="L1403" t="b">
         <v>1</v>
+      </c>
+      <c r="M1403" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1404" spans="1:13" x14ac:dyDescent="0.35">
@@ -47317,6 +47620,9 @@
       <c r="L1409" t="b">
         <v>1</v>
       </c>
+      <c r="M1409" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1410" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1410" t="s">
@@ -47349,6 +47655,9 @@
       <c r="L1410" t="b">
         <v>1</v>
       </c>
+      <c r="M1410" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1411" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1411" t="s">
@@ -47381,6 +47690,9 @@
       <c r="L1411" t="b">
         <v>1</v>
       </c>
+      <c r="M1411" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1412" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1412" t="s">
@@ -47536,6 +47848,9 @@
       <c r="L1415" t="b">
         <v>1</v>
       </c>
+      <c r="M1415" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1416" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1416" t="s">
@@ -47650,6 +47965,9 @@
       <c r="L1418" t="b">
         <v>1</v>
       </c>
+      <c r="M1418" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1419" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1419" t="s">
@@ -47682,6 +48000,9 @@
       <c r="L1419" t="b">
         <v>1</v>
       </c>
+      <c r="M1419" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1420" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1420" t="s">
@@ -47801,6 +48122,9 @@
       <c r="L1423" t="b">
         <v>1</v>
       </c>
+      <c r="M1423" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1424" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1424" t="s">
@@ -47831,6 +48155,9 @@
         <v>0</v>
       </c>
       <c r="L1424" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1424" t="b">
         <v>1</v>
       </c>
     </row>
@@ -48395,6 +48722,9 @@
       <c r="L1438" t="b">
         <v>1</v>
       </c>
+      <c r="M1438" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1439" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1439" t="s">
@@ -48427,6 +48757,9 @@
       <c r="L1439" t="b">
         <v>1</v>
       </c>
+      <c r="M1439" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1440" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1440" t="s">
@@ -48465,6 +48798,9 @@
       <c r="L1440" t="b">
         <v>1</v>
       </c>
+      <c r="M1440" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1441" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1441" t="s">
@@ -48749,6 +49085,9 @@
       <c r="L1447" t="b">
         <v>1</v>
       </c>
+      <c r="M1447" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1448" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1448" t="s">
@@ -48945,6 +49284,9 @@
       <c r="L1452" t="b">
         <v>1</v>
       </c>
+      <c r="M1452" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1453" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1453" t="s">
@@ -48977,6 +49319,9 @@
       <c r="L1453" t="b">
         <v>1</v>
       </c>
+      <c r="M1453" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1454" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1454" t="s">
@@ -49009,6 +49354,9 @@
       <c r="L1454" t="b">
         <v>1</v>
       </c>
+      <c r="M1454" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1455" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1455" t="s">
@@ -49129,6 +49477,9 @@
       <c r="L1457" t="b">
         <v>1</v>
       </c>
+      <c r="M1457" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1458" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1458" t="s">
@@ -49372,6 +49723,9 @@
       <c r="L1463" t="b">
         <v>1</v>
       </c>
+      <c r="M1463" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1464" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1464" t="s">
@@ -49403,6 +49757,9 @@
       </c>
       <c r="L1464" t="b">
         <v>1</v>
+      </c>
+      <c r="M1464" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1465" spans="1:13" x14ac:dyDescent="0.35">
@@ -49518,6 +49875,9 @@
       <c r="L1467" t="b">
         <v>1</v>
       </c>
+      <c r="M1467" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1468" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1468" t="s">
@@ -49550,6 +49910,9 @@
       <c r="L1468" t="b">
         <v>1</v>
       </c>
+      <c r="M1468" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1469" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1469" t="s">
@@ -49582,6 +49945,9 @@
       <c r="L1469" t="b">
         <v>1</v>
       </c>
+      <c r="M1469" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1470" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1470" t="s">
@@ -49702,6 +50068,9 @@
       <c r="L1472" t="b">
         <v>1</v>
       </c>
+      <c r="M1472" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1473" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1473" t="s">
@@ -49980,6 +50349,9 @@
       <c r="L1479" t="b">
         <v>1</v>
       </c>
+      <c r="M1479" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1480" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1480" t="s">
@@ -50434,6 +50806,9 @@
         <v>0</v>
       </c>
       <c r="L1494" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1494" t="b">
         <v>1</v>
       </c>
     </row>
@@ -50474,6 +50849,9 @@
       <c r="L1495" t="b">
         <v>1</v>
       </c>
+      <c r="M1495" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1496" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1496" t="s">
@@ -50887,6 +51265,9 @@
         <v>0</v>
       </c>
       <c r="L1509" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1509" t="b">
         <v>1</v>
       </c>
     </row>
@@ -52006,6 +52387,9 @@
       <c r="L1544" t="b">
         <v>1</v>
       </c>
+      <c r="M1544" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1545" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1545" t="s">
@@ -52038,6 +52422,9 @@
       <c r="L1545" t="b">
         <v>1</v>
       </c>
+      <c r="M1545" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1546" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1546" t="s">
@@ -52070,6 +52457,9 @@
       <c r="L1546" t="b">
         <v>1</v>
       </c>
+      <c r="M1546" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1547" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1547" t="s">
@@ -52102,6 +52492,9 @@
       <c r="L1547" t="b">
         <v>1</v>
       </c>
+      <c r="M1547" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1548" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1548" t="s">
@@ -52134,6 +52527,9 @@
       <c r="L1548" t="b">
         <v>1</v>
       </c>
+      <c r="M1548" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1549" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1549" t="s">
@@ -52171,6 +52567,9 @@
       </c>
       <c r="L1549" t="b">
         <v>1</v>
+      </c>
+      <c r="M1549" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1550" spans="1:13" x14ac:dyDescent="0.35">
@@ -52516,6 +52915,9 @@
       <c r="L1559" t="b">
         <v>1</v>
       </c>
+      <c r="M1559" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1560" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1560" t="s">
@@ -52548,6 +52950,9 @@
       <c r="L1560" t="b">
         <v>1</v>
       </c>
+      <c r="M1560" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1561" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1561" t="s">
@@ -52580,6 +52985,9 @@
       <c r="L1561" t="b">
         <v>1</v>
       </c>
+      <c r="M1561" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1562" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1562" t="s">
@@ -52612,6 +53020,9 @@
       <c r="L1562" t="b">
         <v>1</v>
       </c>
+      <c r="M1562" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1563" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1563" t="s">
@@ -52644,6 +53055,9 @@
       <c r="L1563" t="b">
         <v>1</v>
       </c>
+      <c r="M1563" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1564" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1564" t="s">
@@ -52682,6 +53096,9 @@
       <c r="L1564" t="b">
         <v>1</v>
       </c>
+      <c r="M1564" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="1565" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1565" t="s">
@@ -52901,6 +53318,9 @@
       <c r="L1570" t="b">
         <v>1</v>
       </c>
+      <c r="M1570" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1571" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1571" t="s">
@@ -53019,6 +53439,9 @@
         <v>0</v>
       </c>
       <c r="L1573" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1573" t="b">
         <v>1</v>
       </c>
     </row>
@@ -53486,6 +53909,9 @@
       <c r="L1585" t="b">
         <v>1</v>
       </c>
+      <c r="M1585" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1586" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1586" t="s">
@@ -54033,6 +54459,9 @@
       <c r="L1599" t="b">
         <v>1</v>
       </c>
+      <c r="M1599" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1600" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1600" t="s">
@@ -54316,6 +54745,9 @@
       </c>
       <c r="L1606" t="b">
         <v>1</v>
+      </c>
+      <c r="M1606" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1607" spans="1:13" x14ac:dyDescent="0.35">
@@ -54618,6 +55050,9 @@
       <c r="L1614" t="b">
         <v>1</v>
       </c>
+      <c r="M1614" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1615" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1615" t="s">
@@ -54697,6 +55132,9 @@
       <c r="L1616" t="b">
         <v>1</v>
       </c>
+      <c r="M1616" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1617" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1617" t="s">
@@ -54899,6 +55337,9 @@
       <c r="L1621" t="b">
         <v>1</v>
       </c>
+      <c r="M1621" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1622" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1622" t="s">
@@ -54978,6 +55419,9 @@
       <c r="L1623" t="b">
         <v>1</v>
       </c>
+      <c r="M1623" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1624" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1624" t="s">
@@ -55243,6 +55687,9 @@
       <c r="L1631" t="b">
         <v>1</v>
       </c>
+      <c r="M1631" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1632" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1632" t="s">
@@ -55275,6 +55722,9 @@
       <c r="L1632" t="b">
         <v>1</v>
       </c>
+      <c r="M1632" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1633" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1633" t="s">
@@ -55305,6 +55755,9 @@
         <v>0</v>
       </c>
       <c r="L1633" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1633" t="b">
         <v>1</v>
       </c>
     </row>
@@ -55702,6 +56155,9 @@
       <c r="L1646" t="b">
         <v>1</v>
       </c>
+      <c r="M1646" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1647" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1647" t="s">
@@ -55734,6 +56190,9 @@
       <c r="L1647" t="b">
         <v>1</v>
       </c>
+      <c r="M1647" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="1648" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1648" t="s">
@@ -55764,6 +56223,9 @@
         <v>0</v>
       </c>
       <c r="L1648" t="b">
+        <v>1</v>
+      </c>
+      <c r="M1648" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>